<commit_message>
did a small change with work division
</commit_message>
<xml_diff>
--- a/Documentation/WorkDivision.xlsx
+++ b/Documentation/WorkDivision.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocelle\Desktop\SWD606\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111C3441-0D88-4F3B-B2A7-6A30D8244D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0606FF1D-91B4-4062-94CB-CF72FFE2419C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -221,6 +221,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -290,55 +297,55 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50:N50"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,74 +753,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10" t="s">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -828,100 +835,100 @@
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7">
+      <c r="B6" s="3"/>
+      <c r="C6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="5">
         <v>44833</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L8" s="4"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>44834</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="6">
         <v>0.01</v>
       </c>
@@ -930,62 +937,62 @@
         <v>8</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="4"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>44833</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
         <v>44834</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="5"/>
       <c r="I13" s="6">
         <v>1</v>
       </c>
@@ -998,136 +1005,136 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="13"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="13"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1142,16 +1149,16 @@
       <c r="N21" s="8"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="8"/>
@@ -1160,82 +1167,82 @@
       <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="13"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="1"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1250,16 +1257,16 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="8"/>
@@ -1268,88 +1275,88 @@
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="13"/>
+      <c r="B32" s="1"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="4"/>
@@ -1358,368 +1365,507 @@
       <c r="N33" s="6"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="13"/>
+      <c r="B35" s="1"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="13"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="9"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="285">
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="C47:N47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="A10:B12"/>
+    <mergeCell ref="C10:D12"/>
+    <mergeCell ref="E10:F12"/>
+    <mergeCell ref="G10:H12"/>
+    <mergeCell ref="I10:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A9:B9"/>
@@ -1744,206 +1890,67 @@
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="A10:B12"/>
-    <mergeCell ref="C10:D12"/>
-    <mergeCell ref="E10:F12"/>
-    <mergeCell ref="G10:H12"/>
-    <mergeCell ref="I10:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="C47:N47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:N4 M6:M12 M14:M20 M22:M26 M28:M36">
     <cfRule type="dataBar" priority="2">

</xml_diff>

<commit_message>
added sql file and updated work division
</commit_message>
<xml_diff>
--- a/Documentation/WorkDivision.xlsx
+++ b/Documentation/WorkDivision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocelle\Desktop\SWD606\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A2E5AB-B9CD-4B5A-BB81-B07D2BBBB4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119D0149-5B6C-405F-91E5-51F8D9BF6662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Work Division (Group III)</t>
   </si>
@@ -306,7 +306,40 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -315,58 +348,25 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:J33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,38 +774,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
@@ -838,82 +838,82 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="2">
+      <c r="D6" s="21"/>
+      <c r="E6" s="13">
         <v>44833</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="14" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="9" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
@@ -922,78 +922,78 @@
         <v>15</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2">
+      <c r="D10" s="12"/>
+      <c r="E10" s="13">
         <v>44834</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14">
         <v>0.01</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="14" t="s">
+      <c r="J10" s="14"/>
+      <c r="K10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="14"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="1" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="9" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="9"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
@@ -1002,42 +1002,42 @@
         <v>13</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="2">
+      <c r="D13" s="9"/>
+      <c r="E13" s="13">
         <v>44833</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
+      <c r="F13" s="13"/>
+      <c r="G13" s="13">
         <v>44834</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3">
+      <c r="H13" s="13"/>
+      <c r="I13" s="14">
         <v>1</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="14" t="s">
+      <c r="J13" s="14"/>
+      <c r="K13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1048,32 +1048,38 @@
         <v>17</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="C15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13">
+        <v>44841</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13">
+        <v>44841</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1084,32 +1090,32 @@
         <v>19</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -1120,144 +1126,146 @@
         <v>21</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="C19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2">
+      <c r="D21" s="10"/>
+      <c r="E21" s="13">
         <v>44840</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -1268,100 +1276,102 @@
         <v>28</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="2">
+      <c r="D30" s="10"/>
+      <c r="E30" s="13">
         <v>44836</v>
       </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="C31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="12"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -1372,58 +1382,58 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="5"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
@@ -1434,14 +1444,14 @@
         <v>37</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
@@ -1452,14 +1462,14 @@
         <v>38</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
@@ -1484,10 +1494,10 @@
       <c r="N38" s="5"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="10"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1646,10 +1656,10 @@
       <c r="N47" s="5"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="10"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -1680,8 +1690,8 @@
       <c r="N49" s="5"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -1713,6 +1723,274 @@
     </row>
   </sheetData>
   <mergeCells count="292">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="C48:N48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="C6:D8"/>
+    <mergeCell ref="E6:F8"/>
+    <mergeCell ref="G6:H8"/>
+    <mergeCell ref="I6:J8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C28:N28"/>
+    <mergeCell ref="C39:N39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="C10:D12"/>
+    <mergeCell ref="E10:F12"/>
+    <mergeCell ref="G10:H12"/>
+    <mergeCell ref="I10:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="I29:J29"/>
@@ -1737,274 +2015,6 @@
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="A10:B12"/>
-    <mergeCell ref="C10:D12"/>
-    <mergeCell ref="E10:F12"/>
-    <mergeCell ref="G10:H12"/>
-    <mergeCell ref="I10:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="C6:D8"/>
-    <mergeCell ref="E6:F8"/>
-    <mergeCell ref="G6:H8"/>
-    <mergeCell ref="I6:J8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="C28:N28"/>
-    <mergeCell ref="C39:N39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="C48:N48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
   </mergeCells>
   <conditionalFormatting sqref="M3:N4 M6:M12 M14:M21 M23:M27 M29:M37">
     <cfRule type="dataBar" priority="2">

</xml_diff>